<commit_message>
Relocated pins for easier routing.  I also marked the one stray VIN_HEADER pin on JX2 as no-connect.
</commit_message>
<xml_diff>
--- a/pinmap/microzed_pinout.xlsx
+++ b/pinmap/microzed_pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robma\Documents\Work\ilemt_fpga\pinmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A09F9C-CA31-492C-B499-7089E1B8F7A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03588E7E-5F22-4884-9168-43F648D94CD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2112" yWindow="516" windowWidth="18228" windowHeight="20052" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="2976" windowWidth="19284" windowHeight="22188" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="microzed_pinout" sheetId="1" r:id="rId1"/>
@@ -2833,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5861,7 +5861,7 @@
         <v>644</v>
       </c>
       <c r="D113" t="s">
-        <v>111</v>
+        <v>645</v>
       </c>
       <c r="E113" t="s">
         <v>136</v>

</xml_diff>